<commit_message>
Updated to ext-lt.map and table used in flight-deck briefing
</commit_message>
<xml_diff>
--- a/src/assets/a32nx-briefing/ExtLt-Table.xlsx
+++ b/src/assets/a32nx-briefing/ExtLt-Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_DEV\flybywire-docs\src\assets\a32nx-briefing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4124DAE0-DEEC-441F-AEDA-404DF8DBDF12}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2334FBF7-A030-4757-8280-1A8487007B34}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8205" yWindow="555" windowWidth="37065" windowHeight="15585" xr2:uid="{415B9321-F600-47B0-8A95-2E87AAF4A71E}"/>
+    <workbookView xWindow="10950" yWindow="615" windowWidth="32490" windowHeight="20295" xr2:uid="{415B9321-F600-47B0-8A95-2E87AAF4A71E}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="42">
   <si>
     <t>At gate</t>
   </si>
@@ -105,9 +105,6 @@
     <t>Above 10 000 ft</t>
   </si>
   <si>
-    <t>Up to 10 000 ft</t>
-  </si>
-  <si>
     <t>Below 10 000 ft</t>
   </si>
   <si>
@@ -147,9 +144,6 @@
     <t xml:space="preserve"> Above 10 000 ft</t>
   </si>
   <si>
-    <t xml:space="preserve"> Up to 10 000 ft</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Below 10 000 ft</t>
   </si>
   <si>
@@ -157,6 +151,15 @@
   </si>
   <si>
     <t xml:space="preserve"> Taxi in</t>
+  </si>
+  <si>
+    <t>Initial Climb (clean)</t>
+  </si>
+  <si>
+    <t>Gear Down</t>
+  </si>
+  <si>
+    <t>ON when inspecting ice on wings</t>
   </si>
 </sst>
 </file>
@@ -530,7 +533,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -544,9 +547,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -566,9 +566,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -597,8 +594,11 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -627,13 +627,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>23</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>368740</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>178849</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
+      <xdr:col>33</xdr:col>
       <xdr:colOff>479270</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>49742</xdr:rowOff>
@@ -671,13 +671,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>25</xdr:col>
+      <xdr:col>26</xdr:col>
       <xdr:colOff>523228</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>5172</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
+      <xdr:col>31</xdr:col>
       <xdr:colOff>6364</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>9559</xdr:rowOff>
@@ -1013,24 +1013,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9366AA0-51FC-4F80-8A6A-9C72629B3271}">
-  <dimension ref="A1:O28"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" style="19" customWidth="1"/>
-    <col min="3" max="14" width="6.5703125" customWidth="1"/>
-    <col min="15" max="15" width="1.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" style="18" customWidth="1"/>
+    <col min="3" max="15" width="6.5703125" customWidth="1"/>
+    <col min="16" max="16" width="1.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:15" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:16" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="15"/>
+      <c r="B2" s="14"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -1044,332 +1044,355 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
-    </row>
-    <row r="3" spans="1:15" s="25" customFormat="1" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="23"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="33" t="s">
+      <c r="P2" s="1"/>
+    </row>
+    <row r="3" spans="1:16" s="24" customFormat="1" ht="105.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="22"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="E3" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="F3" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="G3" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="33" t="s">
+      <c r="H3" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="33" t="s">
+      <c r="I3" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="36" t="s">
+      <c r="K3" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="M3" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="J3" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="K3" s="33" t="s">
+      <c r="N3" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="M3" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="N3" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="O3" s="23"/>
-    </row>
-    <row r="4" spans="1:15" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="O3" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="P3" s="22"/>
+    </row>
+    <row r="4" spans="1:16" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="K4" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="L4" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="M4" s="27" t="s">
+      <c r="F4" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="N4" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="N4" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="O4" s="1"/>
-    </row>
-    <row r="5" spans="1:15" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="O4" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="P4" s="1"/>
+    </row>
+    <row r="5" spans="1:16" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A5" s="1"/>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="J5" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="K5" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="L5" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="M5" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="N5" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="O5" s="1"/>
-    </row>
-    <row r="6" spans="1:15" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="C5" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="M5" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="N5" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="O5" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="P5" s="1"/>
+    </row>
+    <row r="6" spans="1:16" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A6" s="1"/>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="26"/>
-      <c r="N6" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="O6" s="1"/>
-    </row>
-    <row r="7" spans="1:15" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="C6" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="P6" s="1"/>
+    </row>
+    <row r="7" spans="1:16" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A7" s="1"/>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="K7" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="L7" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="M7" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="N7" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="O7" s="1"/>
-    </row>
-    <row r="8" spans="1:15" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="C7" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="L7" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="M7" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="N7" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="O7" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="P7" s="1"/>
+    </row>
+    <row r="8" spans="1:16" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A8" s="1"/>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="J8" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="K8" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="L8" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="M8" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="N8" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="O8" s="1"/>
-    </row>
-    <row r="9" spans="1:15" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="C8" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="L8" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="M8" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="N8" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="O8" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="P8" s="1"/>
+    </row>
+    <row r="9" spans="1:16" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A9" s="1"/>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="K9" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="L9" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="M9" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="N9" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="O9" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="P9" s="1"/>
+    </row>
+    <row r="10" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="1"/>
+      <c r="B10" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="I9" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="J9" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="K9" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="L9" s="27" t="s">
+      <c r="C10" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="K10" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="L10" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="M10" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="M9" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="N9" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="O9" s="1"/>
-    </row>
-    <row r="10" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="1"/>
-      <c r="B10" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="G10" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="J10" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="K10" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="L10" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="M10" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="N10" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="O10" s="1"/>
-    </row>
-    <row r="11" spans="1:15" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="N10" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="O10" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="P10" s="1"/>
+    </row>
+    <row r="11" spans="1:16" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A11" s="1"/>
-      <c r="B11" s="18"/>
+      <c r="B11" s="17"/>
       <c r="C11" s="4" t="s">
         <v>20</v>
       </c>
@@ -1382,15 +1405,16 @@
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="O11" s="1"/>
-    </row>
-    <row r="12" spans="1:15" ht="5.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="M11" s="3"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="P11" s="1"/>
+    </row>
+    <row r="12" spans="1:16" ht="5.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="1"/>
-      <c r="B12" s="18"/>
+      <c r="B12" s="17"/>
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
       <c r="E12" s="3"/>
@@ -1403,11 +1427,12 @@
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
-      <c r="O12" s="1"/>
-    </row>
-    <row r="17" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O12" s="3"/>
+      <c r="P12" s="1"/>
+    </row>
+    <row r="17" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
-      <c r="B17" s="15"/>
+      <c r="B17" s="14"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1421,10 +1446,11 @@
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
-    </row>
-    <row r="18" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="P17" s="1"/>
+    </row>
+    <row r="18" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A18" s="1"/>
-      <c r="B18" s="20"/>
+      <c r="B18" s="19"/>
       <c r="C18" s="7" t="s">
         <v>0</v>
       </c>
@@ -1432,7 +1458,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F18" s="7" t="s">
         <v>21</v>
@@ -1443,29 +1469,28 @@
       <c r="H18" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I18" s="7" t="s">
-        <v>23</v>
-      </c>
+      <c r="I18" s="7"/>
       <c r="J18" s="7" t="s">
         <v>22</v>
       </c>
       <c r="K18" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="L18" s="7" t="s">
+      <c r="N18" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="M18" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="N18" s="8" t="s">
+      <c r="O18" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="O18" s="1"/>
-    </row>
-    <row r="19" spans="1:15" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="P18" s="1"/>
+    </row>
+    <row r="19" spans="1:16" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A19" s="1"/>
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="20" t="s">
         <v>16</v>
       </c>
       <c r="C19" s="5" t="s">
@@ -1483,14 +1508,15 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
-      <c r="N19" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="O19" s="1"/>
-    </row>
-    <row r="20" spans="1:15" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="N19" s="5"/>
+      <c r="O19" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="P19" s="1"/>
+    </row>
+    <row r="20" spans="1:16" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A20" s="1"/>
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="20" t="s">
         <v>5</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -1506,14 +1532,15 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
-      <c r="N20" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="O20" s="1"/>
-    </row>
-    <row r="21" spans="1:15" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="N20" s="2"/>
+      <c r="O20" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="P20" s="1"/>
+    </row>
+    <row r="21" spans="1:16" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A21" s="1"/>
-      <c r="B21" s="21" t="s">
+      <c r="B21" s="20" t="s">
         <v>6</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -1530,40 +1557,42 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
-      <c r="M21" s="2" t="s">
+      <c r="M21" s="2"/>
+      <c r="N21" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N21" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="O21" s="1"/>
-    </row>
-    <row r="22" spans="1:15" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="O21" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="P21" s="1"/>
+    </row>
+    <row r="22" spans="1:16" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A22" s="1"/>
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="O22" s="1"/>
-    </row>
-    <row r="23" spans="1:15" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="D22" s="35"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="35"/>
+      <c r="J22" s="35"/>
+      <c r="K22" s="35"/>
+      <c r="L22" s="35"/>
+      <c r="M22" s="35"/>
+      <c r="N22" s="35"/>
+      <c r="O22" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="P22" s="1"/>
+    </row>
+    <row r="23" spans="1:16" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A23" s="1"/>
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="20" t="s">
         <v>8</v>
       </c>
       <c r="C23" s="2" t="s">
@@ -1590,17 +1619,18 @@
         <v>10</v>
       </c>
       <c r="L23" s="2"/>
-      <c r="M23" s="2" t="s">
+      <c r="M23" s="2"/>
+      <c r="N23" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N23" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="O23" s="1"/>
-    </row>
-    <row r="24" spans="1:15" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="O23" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="P23" s="1"/>
+    </row>
+    <row r="24" spans="1:16" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A24" s="1"/>
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="20" t="s">
         <v>17</v>
       </c>
       <c r="C24" s="2" t="s">
@@ -1615,25 +1645,24 @@
         <v>14</v>
       </c>
       <c r="H24" s="2"/>
-      <c r="I24" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
-      <c r="L24" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="L24" s="2"/>
       <c r="M24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N24" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="N24" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="O24" s="1"/>
-    </row>
-    <row r="25" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="O24" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="P24" s="1"/>
+    </row>
+    <row r="25" spans="1:16" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A25" s="1"/>
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="21" t="s">
         <v>18</v>
       </c>
       <c r="C25" s="6" t="s">
@@ -1653,18 +1682,19 @@
       <c r="K25" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L25" s="6" t="s">
+      <c r="L25" s="6"/>
+      <c r="M25" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="M25" s="6"/>
-      <c r="N25" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="O25" s="1"/>
-    </row>
-    <row r="26" spans="1:15" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="N25" s="6"/>
+      <c r="O25" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="P25" s="1"/>
+    </row>
+    <row r="26" spans="1:16" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A26" s="1"/>
-      <c r="B26" s="18"/>
+      <c r="B26" s="17"/>
       <c r="C26" s="4" t="s">
         <v>20</v>
       </c>
@@ -1679,11 +1709,12 @@
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
-      <c r="O26" s="1"/>
-    </row>
-    <row r="27" spans="1:15" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="O26" s="3"/>
+      <c r="P26" s="1"/>
+    </row>
+    <row r="27" spans="1:16" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A27" s="1"/>
-      <c r="B27" s="18"/>
+      <c r="B27" s="17"/>
       <c r="C27" s="4" t="s">
         <v>19</v>
       </c>
@@ -1698,11 +1729,12 @@
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
-      <c r="O27" s="1"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O27" s="3"/>
+      <c r="P27" s="1"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
-      <c r="B28" s="15"/>
+      <c r="B28" s="14"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -1716,11 +1748,12 @@
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C6:M6"/>
-    <mergeCell ref="C22:M22"/>
+    <mergeCell ref="C6:N6"/>
+    <mergeCell ref="C22:N22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>